<commit_message>
more progress on the .sql file
</commit_message>
<xml_diff>
--- a/Documentation/databasePlan.xlsx
+++ b/Documentation/databasePlan.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
   <si>
     <t>time of call</t>
   </si>
@@ -165,12 +165,18 @@
   </si>
   <si>
     <t>ride request</t>
+  </si>
+  <si>
+    <t>drivers</t>
+  </si>
+  <si>
+    <t>vehicles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,18 +416,21 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,27 +440,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -768,11 +774,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22:H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,11 +786,11 @@
     <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="21.109375" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
@@ -799,671 +805,671 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="9"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17"/>
+      <c r="U2" s="17"/>
+      <c r="V2" s="18"/>
     </row>
     <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="U3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="18"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="21"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="16"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="21"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="18"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="1" t="s">
+      <c r="C11" s="22"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="1" t="s">
+      <c r="F11" s="20"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="16"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="21"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="12"/>
+      <c r="I12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="21"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="21"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="21"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="21"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="1" t="s">
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="21"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="24" t="s">
+      <c r="H18" s="5"/>
+      <c r="I18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="L18" s="12"/>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="14"/>
+      <c r="C20" s="17"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="17"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="8"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="21"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="13"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="20"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="13"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="21"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="3" t="s">
+      <c r="I23" s="12"/>
+      <c r="J23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M23" s="20"/>
-      <c r="N23" s="21"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="21"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="13"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="21"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="3" t="s">
+      <c r="F26" s="12"/>
+      <c r="G26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="6" t="s">
+      <c r="J26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="K26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N26" s="21"/>
+      <c r="N26" s="13"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="21"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="13"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="24"/>
+      <c r="K28" s="24"/>
+      <c r="L28" s="24"/>
+      <c r="M28" s="24"/>
       <c r="N28" s="25"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="21"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="13"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="21"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="13"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="21"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="13"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="K32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="20"/>
-      <c r="N32" s="21"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="13"/>
     </row>
     <row r="33" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="12"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="17">

</xml_diff>

<commit_message>
working with index.php to figure out wordpress, fixed the name of the driver table from driver id in the db plan, pushing commits before moving to my own development branch
</commit_message>
<xml_diff>
--- a/Documentation/databasePlan.xlsx
+++ b/Documentation/databasePlan.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlgro\Documents\CS397\STARRS\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D619E148-0197-4948-AC1E-05D5F1F9F83F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -170,7 +171,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -410,18 +411,39 @@
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -431,28 +453,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -768,11 +769,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="B25" sqref="B25:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,684 +800,674 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="8"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="9"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="23"/>
+      <c r="O2" s="23"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="24"/>
     </row>
     <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="M3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="N3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="P3" s="11" t="s">
+      <c r="P3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="R3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="S3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="T3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="U3" s="11" t="s">
+      <c r="U3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="12" t="s">
+      <c r="V3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="9"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="24"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B7" s="19"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="21"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="25"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="K9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="18"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="19"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="21"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="13"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="1" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="1" t="s">
+      <c r="F11" s="17"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="16"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="25"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="3" t="s">
+      <c r="D12" s="12"/>
+      <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="12"/>
+      <c r="I12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="L12" s="18" t="s">
+      <c r="L12" s="10" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="19"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-      <c r="L13" s="21"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="21"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
+      <c r="L14" s="13"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="21"/>
+      <c r="L15" s="13"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20"/>
-      <c r="K16" s="20"/>
-      <c r="L16" s="21"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="13"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="1" t="s">
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="5"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="21"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="13"/>
     </row>
     <row r="18" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="11" t="s">
+      <c r="F18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="23" t="s">
+      <c r="G18" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="24" t="s">
+      <c r="H18" s="5"/>
+      <c r="I18" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="11" t="s">
+      <c r="J18" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="23" t="s">
+      <c r="K18" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="L18" s="12"/>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20"/>
-      <c r="J19" s="20"/>
-      <c r="K19" s="20"/>
-      <c r="L19" s="20"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="14"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="8"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
-      <c r="L21" s="20"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="21"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="13"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="1" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="18"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="5"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="21"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="13"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="3" t="s">
+      <c r="I23" s="12"/>
+      <c r="J23" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="K23" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L23" s="4" t="s">
+      <c r="L23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M23" s="20"/>
-      <c r="N23" s="21"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="13"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="19"/>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
-      <c r="L24" s="20"/>
-      <c r="M24" s="20"/>
-      <c r="N24" s="21"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="13"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="13"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="21"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="3" t="s">
+      <c r="F26" s="12"/>
+      <c r="G26" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="H26" s="6" t="s">
+      <c r="H26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="6" t="s">
+      <c r="I26" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="6" t="s">
+      <c r="J26" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="K26" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="M26" s="4" t="s">
+      <c r="M26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="N26" s="21"/>
+      <c r="N26" s="13"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="19"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20"/>
-      <c r="I27" s="20"/>
-      <c r="J27" s="20"/>
-      <c r="K27" s="20"/>
-      <c r="L27" s="20"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="21"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="13"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="22"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="22"/>
-      <c r="M28" s="22"/>
-      <c r="N28" s="25"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="21"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="F29" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G29" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="4" t="s">
+      <c r="H29" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="21"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="13"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="19"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="21"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="12"/>
+      <c r="I30" s="12"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="12"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="12"/>
+      <c r="N30" s="13"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="21"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="12"/>
+      <c r="N31" s="13"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="6" t="s">
+      <c r="D32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="6" t="s">
+      <c r="E32" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="6" t="s">
+      <c r="F32" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="6" t="s">
+      <c r="G32" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H32" s="6" t="s">
+      <c r="H32" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="I32" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J32" s="6" t="s">
+      <c r="J32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="K32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="L32" s="4" t="s">
+      <c r="L32" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M32" s="20"/>
-      <c r="N32" s="21"/>
+      <c r="M32" s="12"/>
+      <c r="N32" s="13"/>
     </row>
     <row r="33" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="10"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="12"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="G25:M25"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="I17:K17"/>
     <mergeCell ref="B2:V2"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="B11:C11"/>
@@ -1484,6 +1475,16 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="B6:L6"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="G25:M25"/>
+    <mergeCell ref="B28:H28"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="B31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
renamed old db_config file, new file is now db_config.sql, new file still unstable, use old until stable config file is complete
</commit_message>
<xml_diff>
--- a/Documentation/databasePlan.xlsx
+++ b/Documentation/databasePlan.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlgro\Documents\CS397\STARRS\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8443EE72-60EF-4982-9EBA-B35F7EE51910}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="111">
   <si>
     <t>time of call</t>
   </si>
@@ -113,12 +114,6 @@
     <t>second breakdown</t>
   </si>
   <si>
-    <t>vehicle id</t>
-  </si>
-  <si>
-    <t>*vehicle id</t>
-  </si>
-  <si>
     <t>current oil status</t>
   </si>
   <si>
@@ -140,30 +135,9 @@
     <t>status</t>
   </si>
   <si>
-    <t>driver id</t>
-  </si>
-  <si>
-    <t>driver name</t>
-  </si>
-  <si>
-    <t>*driver id</t>
-  </si>
-  <si>
-    <t>shift id</t>
-  </si>
-  <si>
-    <t>*shift id</t>
-  </si>
-  <si>
-    <t>current anti-freeze status</t>
-  </si>
-  <si>
     <t>current milage</t>
   </si>
   <si>
-    <t>request id</t>
-  </si>
-  <si>
     <t>ride request</t>
   </si>
   <si>
@@ -171,13 +145,226 @@
   </si>
   <si>
     <t>vehicles</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>plateNum</t>
+  </si>
+  <si>
+    <t>mileage</t>
+  </si>
+  <si>
+    <t>oilStatus</t>
+  </si>
+  <si>
+    <t>antifreezeStatus</t>
+  </si>
+  <si>
+    <t>primary key</t>
+  </si>
+  <si>
+    <t>unique</t>
+  </si>
+  <si>
+    <t>auto-incremented</t>
+  </si>
+  <si>
+    <t>first letter t for test, j for jitney, s for shuttle, increment 2 digit number after (ie j01 and j02 for the first and second jitneys)</t>
+  </si>
+  <si>
+    <t>license plate of the vehicle</t>
+  </si>
+  <si>
+    <t>"ok" or "low"</t>
+  </si>
+  <si>
+    <t>50 char small blurb</t>
+  </si>
+  <si>
+    <t>edit vehicles</t>
+  </si>
+  <si>
+    <t>before you leave</t>
+  </si>
+  <si>
+    <t>edit vehicels/extra field?</t>
+  </si>
+  <si>
+    <t>vehicle_ID</t>
+  </si>
+  <si>
+    <t>foreign key 'id' from vehicles</t>
+  </si>
+  <si>
+    <t>milliseconds since 1970 (20 digit integer)</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>double, 11 digits, 7 after decimal</t>
+  </si>
+  <si>
+    <t>see vehicles table</t>
+  </si>
+  <si>
+    <t>logLocation script</t>
+  </si>
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>auto-increment</t>
+  </si>
+  <si>
+    <t>name of driver</t>
+  </si>
+  <si>
+    <t>colby username</t>
+  </si>
+  <si>
+    <t>cobly email</t>
+  </si>
+  <si>
+    <t>100 char blurb</t>
+  </si>
+  <si>
+    <t>edit drivers</t>
+  </si>
+  <si>
+    <t>edit drivers/extra field?</t>
+  </si>
+  <si>
+    <t>shifts</t>
+  </si>
+  <si>
+    <t>driver_ID</t>
+  </si>
+  <si>
+    <t>foreign key 'id' from drivers</t>
+  </si>
+  <si>
+    <t>10 digit int</t>
+  </si>
+  <si>
+    <t>5 digit int</t>
+  </si>
+  <si>
+    <t>2 digit int</t>
+  </si>
+  <si>
+    <t>edit vehicles/before you leave</t>
+  </si>
+  <si>
+    <t>see drivers table</t>
+  </si>
+  <si>
+    <t>edit shifts</t>
+  </si>
+  <si>
+    <t>datetime2 format</t>
+  </si>
+  <si>
+    <t>7 chars</t>
+  </si>
+  <si>
+    <t>shift_ID</t>
+  </si>
+  <si>
+    <t>date format</t>
+  </si>
+  <si>
+    <t>pending/ accepted/ enroute/ complete</t>
+  </si>
+  <si>
+    <t>shift_info</t>
+  </si>
+  <si>
+    <t>milageStart</t>
+  </si>
+  <si>
+    <t>milageFinish</t>
+  </si>
+  <si>
+    <t>fillUpGallons</t>
+  </si>
+  <si>
+    <t>timeOfCall</t>
+  </si>
+  <si>
+    <t>pickupTime</t>
+  </si>
+  <si>
+    <t>dropoffTime</t>
+  </si>
+  <si>
+    <t>pickupLocation</t>
+  </si>
+  <si>
+    <t>dropoffLocation</t>
+  </si>
+  <si>
+    <t>numPeople</t>
+  </si>
+  <si>
+    <t>rideStatus</t>
+  </si>
+  <si>
+    <t>foreign key 'id' from shifts</t>
+  </si>
+  <si>
+    <t>12 digit int</t>
+  </si>
+  <si>
+    <t>when driver accepts call</t>
+  </si>
+  <si>
+    <t>jitney request page</t>
+  </si>
+  <si>
+    <t>when driver indicates a pickup</t>
+  </si>
+  <si>
+    <t>when driver indicates a dropoff</t>
+  </si>
+  <si>
+    <t>100 chars</t>
+  </si>
+  <si>
+    <t>250 chars</t>
+  </si>
+  <si>
+    <t>jitney request page/driver input</t>
+  </si>
+  <si>
+    <t>see shifts tabel for details</t>
+  </si>
+  <si>
+    <t>before you drive</t>
+  </si>
+  <si>
+    <t>7 digit int</t>
+  </si>
+  <si>
+    <t>5 digit double, 3 after decimal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,16 +372,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="21">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -410,11 +623,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -422,8 +653,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
@@ -431,6 +660,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -440,25 +687,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -775,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:V33"/>
+  <dimension ref="B1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:H22"/>
+    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R40" sqref="R40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -805,29 +1087,29 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17"/>
-      <c r="T2" s="17"/>
-      <c r="U2" s="17"/>
-      <c r="V2" s="18"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="21"/>
+      <c r="V2" s="22"/>
     </row>
     <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
@@ -896,50 +1178,50 @@
     </row>
     <row r="5" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="21"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="23"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -969,48 +1251,48 @@
       <c r="K9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L9" s="10"/>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="11"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="23" t="s">
+      <c r="C11" s="17"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="20"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="23" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-      <c r="L11" s="21"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="23"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="10"/>
       <c r="E12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1020,50 +1302,50 @@
       <c r="G12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="10"/>
       <c r="I12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="L12" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="11"/>
+    </row>
+    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="B14" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="K12" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="L12" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-    </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="13"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
+      <c r="L14" s="11"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1093,37 +1375,37 @@
       <c r="K15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="L15" s="13"/>
+      <c r="L15" s="11"/>
     </row>
     <row r="16" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B16" s="11"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="13"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="11"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="23" t="s">
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="20"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="13"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="11"/>
     </row>
     <row r="18" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="4" t="s">
@@ -1139,350 +1421,685 @@
         <v>11</v>
       </c>
       <c r="F18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="5"/>
+      <c r="I18" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="K18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="J18" s="5" t="s">
+      <c r="L18" s="6"/>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B19" s="10"/>
+      <c r="C19" s="10"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="10"/>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B20" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B22" s="29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="30"/>
+      <c r="H22" s="31"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="46"/>
+      <c r="N22" s="10"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B23" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H23" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="10"/>
+      <c r="J23" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="K23" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="M23" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="N23" s="10"/>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B24" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="L24" s="14"/>
+      <c r="M24" s="33"/>
+      <c r="N24" s="10"/>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B25" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="K18" s="14" t="s">
+      <c r="F25" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G25" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H25" s="36" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="10"/>
+      <c r="J25" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="L25" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="M25" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="N25" s="10"/>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="I26" s="10"/>
+      <c r="J26" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="K26" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="L26" s="37" t="s">
+        <v>64</v>
+      </c>
+      <c r="M26" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="N26" s="10"/>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B27" s="10"/>
+      <c r="C27" s="10"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B28" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" s="40"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="41"/>
+      <c r="H28" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="50"/>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F29" s="33" t="s">
+        <v>35</v>
+      </c>
+      <c r="H29" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="K29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M29" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="N29" s="33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B30" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="10"/>
+      <c r="D30" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" s="33"/>
+      <c r="H30" s="42" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="J30" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="33"/>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B31" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" s="42" t="s">
+        <v>76</v>
+      </c>
+      <c r="I31" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="J31" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K31" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="L31" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="M31" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="N31" s="36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B32" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D32" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="I32" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="J32" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="K32" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="M32" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="N32" s="38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B33" s="24"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B34" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="16"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B35" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B36" s="32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
+      <c r="E36" s="10"/>
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="33"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+      <c r="K36" s="10"/>
+      <c r="L36" s="10"/>
+      <c r="M36" s="10"/>
+      <c r="N36" s="10"/>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B37" s="42" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="H37" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="10"/>
+      <c r="M37" s="10"/>
+      <c r="N37" s="10"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B38" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="10"/>
+      <c r="L38" s="10"/>
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="10"/>
+      <c r="E39" s="10"/>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="10"/>
+      <c r="K39" s="10"/>
+      <c r="L39" s="10"/>
+      <c r="M39" s="10"/>
+      <c r="N39" s="10"/>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B40" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="12"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-    </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-      <c r="M20" s="7"/>
-      <c r="N20" s="8"/>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B21" s="11"/>
-      <c r="C21" s="12"/>
-      <c r="D21" s="12"/>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="13"/>
-    </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="22"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="20"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="13"/>
-    </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="H23" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M23" s="12"/>
-      <c r="N23" s="13"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="13"/>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
-      <c r="L25" s="20"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="13"/>
-    </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B26" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F26" s="12"/>
-      <c r="G26" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="16"/>
+      <c r="H40" s="16"/>
+      <c r="I40" s="16"/>
+      <c r="J40" s="16"/>
+      <c r="K40" s="16"/>
+      <c r="L40" s="17"/>
+      <c r="M40" s="10"/>
+      <c r="N40" s="10"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B41" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="I26" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="N26" s="13"/>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B27" s="11"/>
-      <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="13"/>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="24"/>
-      <c r="N28" s="25"/>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="2" t="s">
+      <c r="C41" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="I41" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="12"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="13"/>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="11"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="13"/>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B31" s="19" t="s">
+      <c r="J41" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="K41" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L41" s="33"/>
+      <c r="M41" s="10"/>
+      <c r="N41" s="10"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B42" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="22"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="13"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K32" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M32" s="12"/>
-      <c r="N32" s="13"/>
-    </row>
-    <row r="33" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="4"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="6"/>
+      <c r="C42" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D42" s="10"/>
+      <c r="E42" s="10"/>
+      <c r="F42" s="10"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="10"/>
+      <c r="J42" s="10"/>
+      <c r="K42" s="10"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="10"/>
+      <c r="N42" s="10"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B43" s="42" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E43" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="K43" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="L43" s="33"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B44" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="L44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="G25:M25"/>
-    <mergeCell ref="B28:H28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="B31:L31"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="I17:K17"/>
     <mergeCell ref="B2:V2"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="B11:C11"/>
@@ -1490,6 +2107,16 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="B6:L6"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="I17:K17"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="H28:N28"/>
+    <mergeCell ref="B28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changed the database config file to add a column to ride request to include user and a column to vehicle to indicate is driving. also changed valid fields to enum instead of varchar and relying on valid input. The database plan spreadsheet still needs to be updated
</commit_message>
<xml_diff>
--- a/Documentation/databasePlan.xlsx
+++ b/Documentation/databasePlan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wlgro\Documents\CS397\STARRS\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8443EE72-60EF-4982-9EBA-B35F7EE51910}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6FBADF-A8F9-4E46-9AD3-269A1C59CAFA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -285,9 +285,6 @@
     <t>date format</t>
   </si>
   <si>
-    <t>pending/ accepted/ enroute/ complete</t>
-  </si>
-  <si>
     <t>shift_info</t>
   </si>
   <si>
@@ -358,6 +355,9 @@
   </si>
   <si>
     <t>5 digit double, 3 after decimal</t>
+  </si>
+  <si>
+    <t>pending/ accepted/ enroute/ complete/cancel</t>
   </si>
 </sst>
 </file>
@@ -663,49 +663,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
@@ -717,23 +678,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -741,6 +732,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1059,8 +1059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:V44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R40" sqref="R40"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K43" sqref="K43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,29 +1087,29 @@
   <sheetData>
     <row r="1" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="22"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="33"/>
     </row>
     <row r="3" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
@@ -1178,19 +1178,19 @@
     </row>
     <row r="5" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="6" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="22"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="33"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B7" s="9"/>
@@ -1206,19 +1206,19 @@
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="23"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="36"/>
     </row>
     <row r="9" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B9" s="7" t="s">
@@ -1267,23 +1267,23 @@
       <c r="L10" s="11"/>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="37"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="F11" s="35"/>
+      <c r="G11" s="37"/>
       <c r="H11" s="10"/>
-      <c r="I11" s="18" t="s">
+      <c r="I11" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="23"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="36"/>
     </row>
     <row r="12" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B12" s="7" t="s">
@@ -1330,18 +1330,18 @@
       <c r="L13" s="11"/>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="17"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="37"/>
       <c r="L14" s="11"/>
     </row>
     <row r="15" spans="2:22" x14ac:dyDescent="0.3">
@@ -1391,20 +1391,20 @@
       <c r="L16" s="11"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="37"/>
       <c r="H17" s="10"/>
-      <c r="I17" s="18" t="s">
+      <c r="I17" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="17"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="37"/>
       <c r="L17" s="11"/>
     </row>
     <row r="18" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1452,19 +1452,19 @@
       <c r="L19" s="10"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="19"/>
-      <c r="L20" s="19"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="44"/>
+      <c r="H20" s="44"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
+      <c r="K20" s="44"/>
+      <c r="L20" s="44"/>
       <c r="M20" s="10"/>
       <c r="N20" s="10"/>
     </row>
@@ -1484,26 +1484,26 @@
       <c r="N21" s="10"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="31"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="42"/>
       <c r="I22" s="10"/>
-      <c r="J22" s="44" t="s">
+      <c r="J22" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="K22" s="16"/>
-      <c r="L22" s="16"/>
-      <c r="M22" s="46"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="29"/>
       <c r="N22" s="10"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C23" s="10" t="s">
@@ -1521,11 +1521,11 @@
       <c r="G23" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="H23" s="20" t="s">
         <v>26</v>
       </c>
       <c r="I23" s="10"/>
-      <c r="J23" s="47" t="s">
+      <c r="J23" s="30" t="s">
         <v>56</v>
       </c>
       <c r="K23" s="10" t="s">
@@ -1534,13 +1534,13 @@
       <c r="L23" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="M23" s="36" t="s">
+      <c r="M23" s="23" t="s">
         <v>61</v>
       </c>
       <c r="N23" s="10"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B24" s="34" t="s">
+      <c r="B24" s="21" t="s">
         <v>46</v>
       </c>
       <c r="C24" s="14" t="s">
@@ -1552,20 +1552,20 @@
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
-      <c r="H24" s="35"/>
+      <c r="H24" s="22"/>
       <c r="I24" s="10"/>
-      <c r="J24" s="34" t="s">
+      <c r="J24" s="21" t="s">
         <v>57</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>46</v>
       </c>
       <c r="L24" s="14"/>
-      <c r="M24" s="33"/>
+      <c r="M24" s="20"/>
       <c r="N24" s="10"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="19" t="s">
         <v>78</v>
       </c>
       <c r="C25" s="10" t="s">
@@ -1574,29 +1574,29 @@
       <c r="D25" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G25" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H25" s="36" t="s">
+      <c r="H25" s="23" t="s">
         <v>52</v>
       </c>
       <c r="I25" s="10"/>
-      <c r="J25" s="42" t="s">
+      <c r="J25" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="K25" s="24" t="s">
+      <c r="K25" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="L25" s="24" t="s">
+      <c r="L25" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="M25" s="36" t="s">
+      <c r="M25" s="23" t="s">
         <v>62</v>
       </c>
       <c r="N25" s="10"/>
@@ -1605,35 +1605,35 @@
       <c r="B26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="37" t="s">
+      <c r="C26" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D26" s="37" t="s">
+      <c r="D26" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="37" t="s">
+      <c r="E26" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="37" t="s">
+      <c r="F26" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="G26" s="37" t="s">
+      <c r="G26" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="H26" s="38" t="s">
+      <c r="H26" s="25" t="s">
         <v>55</v>
       </c>
       <c r="I26" s="10"/>
-      <c r="J26" s="43" t="s">
+      <c r="J26" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="K26" s="37" t="s">
+      <c r="K26" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="L26" s="37" t="s">
+      <c r="L26" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="M26" s="38" t="s">
+      <c r="M26" s="25" t="s">
         <v>64</v>
       </c>
       <c r="N26" s="10"/>
@@ -1654,46 +1654,46 @@
       <c r="N27" s="10"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B28" s="39" t="s">
+      <c r="B28" s="48" t="s">
         <v>38</v>
       </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="41"/>
-      <c r="H28" s="48" t="s">
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="50"/>
+      <c r="H28" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="49"/>
-      <c r="L28" s="49"/>
-      <c r="M28" s="49"/>
-      <c r="N28" s="50"/>
+      <c r="I28" s="46"/>
+      <c r="J28" s="46"/>
+      <c r="K28" s="46"/>
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="47"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="19" t="s">
         <v>40</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="15" t="s">
         <v>65</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H29" s="32" t="s">
+      <c r="H29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="I29" s="26" t="s">
+      <c r="I29" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="25" t="s">
+      <c r="J29" s="16" t="s">
         <v>56</v>
       </c>
       <c r="K29" s="10" t="s">
@@ -1705,117 +1705,117 @@
       <c r="M29" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="N29" s="33" t="s">
+      <c r="N29" s="20" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B30" s="42" t="s">
+      <c r="B30" s="26" t="s">
         <v>46</v>
       </c>
       <c r="C30" s="10"/>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="33"/>
-      <c r="H30" s="42" t="s">
+      <c r="F30" s="20"/>
+      <c r="H30" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="I30" s="24" t="s">
+      <c r="I30" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="J30" s="24" t="s">
+      <c r="J30" s="15" t="s">
         <v>57</v>
       </c>
       <c r="K30" s="10"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
-      <c r="N30" s="33"/>
+      <c r="N30" s="20"/>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B31" s="42" t="s">
+      <c r="B31" s="26" t="s">
         <v>77</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="H31" s="42" t="s">
+      <c r="H31" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="I31" s="24" t="s">
+      <c r="I31" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="J31" s="24" t="s">
+      <c r="J31" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="K31" s="24" t="s">
+      <c r="K31" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="L31" s="24" t="s">
+      <c r="L31" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="M31" s="24" t="s">
+      <c r="M31" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="N31" s="36" t="s">
+      <c r="N31" s="23" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="27" t="s">
         <v>66</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="E32" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="F32" s="38" t="s">
+      <c r="F32" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="H32" s="43" t="s">
+      <c r="H32" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="I32" s="37" t="s">
+      <c r="I32" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="J32" s="37" t="s">
+      <c r="J32" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="K32" s="37" t="s">
+      <c r="K32" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="L32" s="37" t="s">
+      <c r="L32" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="M32" s="37" t="s">
+      <c r="M32" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="N32" s="38" t="s">
+      <c r="N32" s="25" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B33" s="24"/>
+      <c r="B33" s="15"/>
       <c r="C33" s="10"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
       <c r="F33" s="10"/>
       <c r="H33" s="10"/>
       <c r="I33" s="10"/>
@@ -1826,34 +1826,34 @@
       <c r="N33" s="10"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B34" s="44" t="s">
+      <c r="B34" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="44"/>
+      <c r="K34" s="44"/>
+      <c r="L34" s="44"/>
+      <c r="M34" s="44"/>
+      <c r="N34" s="44"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B35" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B35" s="45" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="D35" s="10" t="s">
+      <c r="E35" s="10" t="s">
         <v>89</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>90</v>
       </c>
       <c r="F35" s="10" t="s">
         <v>44</v>
@@ -1861,7 +1861,7 @@
       <c r="G35" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H35" s="33" t="s">
+      <c r="H35" s="20" t="s">
         <v>18</v>
       </c>
       <c r="I35" s="10"/>
@@ -1872,15 +1872,15 @@
       <c r="N35" s="10"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B36" s="32" t="s">
-        <v>98</v>
+      <c r="B36" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
-      <c r="H36" s="33"/>
+      <c r="H36" s="20"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
@@ -1889,26 +1889,26 @@
       <c r="N36" s="10"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B37" s="42" t="s">
-        <v>107</v>
+      <c r="B37" s="26" t="s">
+        <v>106</v>
       </c>
       <c r="C37" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E37" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>110</v>
-      </c>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="G37" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="H37" s="36" t="s">
-        <v>105</v>
+      <c r="H37" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
@@ -1918,11 +1918,11 @@
       <c r="N37" s="10"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B38" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" s="37" t="s">
-        <v>108</v>
+      <c r="B38" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>107</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>54</v>
@@ -1947,8 +1947,8 @@
       <c r="N38" s="10"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
       <c r="F39" s="10"/>
@@ -1962,63 +1962,63 @@
       <c r="N39" s="10"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B40" s="44" t="s">
+      <c r="B40" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="16"/>
-      <c r="L40" s="17"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="35"/>
+      <c r="G40" s="35"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="35"/>
+      <c r="J40" s="35"/>
+      <c r="K40" s="35"/>
+      <c r="L40" s="37"/>
       <c r="M40" s="10"/>
       <c r="N40" s="10"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B41" s="32" t="s">
+      <c r="B41" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="18" t="s">
         <v>84</v>
       </c>
       <c r="D41" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="E41" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="F41" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="F41" s="10" t="s">
+      <c r="G41" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G41" s="10" t="s">
+      <c r="H41" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="H41" s="10" t="s">
+      <c r="I41" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="I41" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="J41" s="10" t="s">
+      <c r="K41" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="K41" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="L41" s="33"/>
+      <c r="L41" s="20"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B42" s="32" t="s">
+      <c r="B42" s="19" t="s">
         <v>46</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -2028,15 +2028,15 @@
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
-      <c r="L42" s="33"/>
+      <c r="L42" s="20"/>
       <c r="M42" s="10"/>
       <c r="N42" s="10"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B43" s="42" t="s">
-        <v>99</v>
-      </c>
-      <c r="C43" s="24" t="s">
+      <c r="B43" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" s="15" t="s">
         <v>76</v>
       </c>
       <c r="D43" s="10" t="s">
@@ -2049,57 +2049,67 @@
         <v>82</v>
       </c>
       <c r="G43" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="I43" s="10" t="s">
         <v>104</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>105</v>
       </c>
       <c r="J43" s="10" t="s">
         <v>78</v>
       </c>
       <c r="K43" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="L43" s="33"/>
+        <v>110</v>
+      </c>
+      <c r="L43" s="20"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="F44" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>103</v>
-      </c>
       <c r="G44" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="J44" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K44" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="L44" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="B40:L40"/>
+    <mergeCell ref="H28:N28"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="B20:L20"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="I17:K17"/>
     <mergeCell ref="B2:V2"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="B11:C11"/>
@@ -2107,16 +2117,6 @@
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="I11:L11"/>
     <mergeCell ref="B6:L6"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="B20:L20"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="I17:K17"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="B40:L40"/>
-    <mergeCell ref="H28:N28"/>
-    <mergeCell ref="B28:F28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>